<commit_message>
adding test case and app file within the repo for better maintainace
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationAssignment.xlsx
+++ b/src/test/resources/AutomationAssignment.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Mobile Number</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>ItemSelection</t>
-  </si>
-  <si>
-    <t>8073547939</t>
-  </si>
-  <si>
-    <t>0000000</t>
   </si>
   <si>
     <t>Testing1!</t>
@@ -59,7 +53,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -77,9 +71,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+    </font>
+    <font>
       <sz val="8.0"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -118,27 +116,27 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf quotePrefix="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -384,26 +382,26 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="5">
+        <v>8.073547939E9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3">
@@ -413,7 +411,6 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>